<commit_message>
Conduct S4 tests for 2000 users
</commit_message>
<xml_diff>
--- a/Wyniki 3/Gotowe!/S3.xlsx
+++ b/Wyniki 3/Gotowe!/S3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\OneDrive\Pulpit\Projekty\Praca magisterska\Wyniki 3\Gotowe!\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495DE619-8393-466C-88AB-AFC535700106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A784531B-6A30-459D-B830-1100E4CDE53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -536,10 +536,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -827,7 +827,7 @@
   <dimension ref="G3:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,17 +838,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="7:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" spans="7:15" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="5" t="s">
@@ -880,7 +880,7 @@
       </c>
     </row>
     <row r="5" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>100</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -909,7 +909,7 @@
       </c>
     </row>
     <row r="6" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G6" s="7"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="4" t="s">
         <v>11</v>
       </c>
@@ -936,7 +936,7 @@
       </c>
     </row>
     <row r="7" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G7" s="7"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="4" t="s">
         <v>12</v>
       </c>
@@ -963,7 +963,7 @@
       </c>
     </row>
     <row r="8" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G8" s="7"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="4" t="s">
         <v>13</v>
       </c>
@@ -990,7 +990,7 @@
       </c>
     </row>
     <row r="9" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G9" s="7"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1017,7 +1017,7 @@
       </c>
     </row>
     <row r="10" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G10" s="7"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1044,7 +1044,7 @@
       </c>
     </row>
     <row r="11" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G11" s="7"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1071,7 +1071,7 @@
       </c>
     </row>
     <row r="12" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G12" s="7"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="4" t="s">
         <v>9</v>
       </c>
@@ -1098,7 +1098,7 @@
       </c>
     </row>
     <row r="13" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <v>1000</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -1127,7 +1127,7 @@
       </c>
     </row>
     <row r="14" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G14" s="7"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1154,7 +1154,7 @@
       </c>
     </row>
     <row r="15" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G15" s="7"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="4" t="s">
         <v>12</v>
       </c>
@@ -1181,7 +1181,7 @@
       </c>
     </row>
     <row r="16" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G16" s="7"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="4" t="s">
         <v>13</v>
       </c>
@@ -1208,7 +1208,7 @@
       </c>
     </row>
     <row r="17" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G17" s="7"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="4" t="s">
         <v>6</v>
       </c>
@@ -1235,7 +1235,7 @@
       </c>
     </row>
     <row r="18" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G18" s="7"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="4" t="s">
         <v>7</v>
       </c>
@@ -1262,7 +1262,7 @@
       </c>
     </row>
     <row r="19" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G19" s="7"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="4" t="s">
         <v>8</v>
       </c>
@@ -1289,7 +1289,7 @@
       </c>
     </row>
     <row r="20" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G20" s="7"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="4" t="s">
         <v>9</v>
       </c>
@@ -1316,7 +1316,7 @@
       </c>
     </row>
     <row r="21" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>4000</v>
       </c>
       <c r="H21" s="4" t="s">
@@ -1345,7 +1345,7 @@
       </c>
     </row>
     <row r="22" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G22" s="7"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="4" t="s">
         <v>11</v>
       </c>
@@ -1372,7 +1372,7 @@
       </c>
     </row>
     <row r="23" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G23" s="7"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="4" t="s">
         <v>12</v>
       </c>
@@ -1399,7 +1399,7 @@
       </c>
     </row>
     <row r="24" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G24" s="7"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="4" t="s">
         <v>13</v>
       </c>
@@ -1426,7 +1426,7 @@
       </c>
     </row>
     <row r="25" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G25" s="7"/>
+      <c r="G25" s="6"/>
       <c r="H25" s="4" t="s">
         <v>6</v>
       </c>
@@ -1453,7 +1453,7 @@
       </c>
     </row>
     <row r="26" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G26" s="7"/>
+      <c r="G26" s="6"/>
       <c r="H26" s="4" t="s">
         <v>7</v>
       </c>
@@ -1480,7 +1480,7 @@
       </c>
     </row>
     <row r="27" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G27" s="7"/>
+      <c r="G27" s="6"/>
       <c r="H27" s="4" t="s">
         <v>8</v>
       </c>
@@ -1507,7 +1507,7 @@
       </c>
     </row>
     <row r="28" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G28" s="7"/>
+      <c r="G28" s="6"/>
       <c r="H28" s="4" t="s">
         <v>9</v>
       </c>

</xml_diff>